<commit_message>
Build site at 2023-03-17 16:19:35 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOT2038.xlsx
+++ b/assets/disciplinas/LOT2038.xlsx
@@ -127,11 +127,11 @@
     <t>Requisitos:</t>
   </si>
   <si>
+    <t xml:space="preserve">LOT2028 -  Tecnologia de Processos Fermentativos  (Requisito fraco)
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">LOT2052 -  Tecnologia de Bebidas Experimental  (Indicação de Conjunto)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOT2028 -  Tecnologia de Processos Fermentativos  (Requisito fraco)
 </t>
   </si>
 </sst>

</xml_diff>